<commit_message>
fixed question prompt, sample steps
</commit_message>
<xml_diff>
--- a/data/Question Bank-1718.xlsx
+++ b/data/Question Bank-1718.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tr246\Desktop\Robotics\Github repository\StepWise\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0ACF06E3-00F0-4B20-9421-048E29B8C220}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B92A7BB1-2A96-4373-86A1-61090F077CF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{ED039E2A-197B-4D3F-A7CF-8E180684E428}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="164">
   <si>
     <t>Subject</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -732,6 +732,10 @@
   </si>
   <si>
     <t>[['OK', 1]]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Prompt</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -772,6 +776,7 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Aptos Display"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1565,8 +1570,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49E4F672-86DF-4215-A992-0B55EA850FA8}">
   <dimension ref="A1:J33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21:E33"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1604,7 +1609,7 @@
         <v>43</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>2</v>
+        <v>163</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>44</v>
@@ -2884,12 +2889,11 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="e8d361d9-3733-4d63-a352-ddfb273e54a3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3087,17 +3091,26 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="e8d361d9-3733-4d63-a352-ddfb273e54a3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C9D1614B-3063-4D46-85D3-79EF77552796}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{50F6A043-8B0C-47F4-B4B7-BEC9D68F34E5}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="e8d361d9-3733-4d63-a352-ddfb273e54a3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -3121,17 +3134,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{50F6A043-8B0C-47F4-B4B7-BEC9D68F34E5}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C9D1614B-3063-4D46-85D3-79EF77552796}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="e8d361d9-3733-4d63-a352-ddfb273e54a3"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>